<commit_message>
Actualizar configuración de VSCode, mejorar la lógica de creación de empleados y agregar clase WaitUtil para manejo de loaders
</commit_message>
<xml_diff>
--- a/src/test/resources/datos.xlsx
+++ b/src/test/resources/datos.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jose.ladino\Automatizacion\ProjectMaven\automatizacion\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jose.ladino\Automatizacion\ProjectMaven\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE11E7F-CBCB-409E-B80E-A2CDF8A7DBEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE042979-1C38-43BD-9B45-A9F67492C42C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-1815" windowWidth="29040" windowHeight="15720" xr2:uid="{1B2942B2-1002-49AC-B066-AD15A2B34D50}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="99">
   <si>
     <t>Estado</t>
   </si>
@@ -241,13 +241,93 @@
   </si>
   <si>
     <t>David</t>
+  </si>
+  <si>
+    <t>2001-04-24</t>
+  </si>
+  <si>
+    <t>2001-05-24</t>
+  </si>
+  <si>
+    <t>2001-06-24</t>
+  </si>
+  <si>
+    <t>2001-04-25</t>
+  </si>
+  <si>
+    <t>2001-05-25</t>
+  </si>
+  <si>
+    <t>2001-06-25</t>
+  </si>
+  <si>
+    <t>2001-04-26</t>
+  </si>
+  <si>
+    <t>2001-05-26</t>
+  </si>
+  <si>
+    <t>2001-06-26</t>
+  </si>
+  <si>
+    <t>2019-02-24</t>
+  </si>
+  <si>
+    <t>2019-04-24</t>
+  </si>
+  <si>
+    <t>2019-05-24</t>
+  </si>
+  <si>
+    <t>2019-06-24</t>
+  </si>
+  <si>
+    <t>2019-02-25</t>
+  </si>
+  <si>
+    <t>2019-04-25</t>
+  </si>
+  <si>
+    <t>2019-05-25</t>
+  </si>
+  <si>
+    <t>2019-06-25</t>
+  </si>
+  <si>
+    <t>2019-02-26</t>
+  </si>
+  <si>
+    <t>Lorena</t>
+  </si>
+  <si>
+    <t>Jimmy</t>
+  </si>
+  <si>
+    <t>Patricia</t>
+  </si>
+  <si>
+    <t>Melissa</t>
+  </si>
+  <si>
+    <t>Joaquin</t>
+  </si>
+  <si>
+    <t>Pilar</t>
+  </si>
+  <si>
+    <t>Lourdes</t>
+  </si>
+  <si>
+    <t>Joseph</t>
+  </si>
+  <si>
+    <t>Melina</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -620,71 +700,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55EA86F-2CF4-4D61-97BB-1D094DEA001F}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.5703125"/>
-    <col min="2" max="2" customWidth="true" width="21.7109375"/>
-    <col min="3" max="3" customWidth="true" width="16.7109375"/>
-    <col min="4" max="4" customWidth="true" width="13.140625"/>
-    <col min="5" max="5" customWidth="true" width="21.5703125"/>
-    <col min="6" max="10" customWidth="true" width="25.28515625"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" customWidth="1"/>
+    <col min="6" max="10" width="25.28515625" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="H1" t="s" s="0">
+      <c r="H1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" t="s" s="0">
+      <c r="I1" t="s">
         <v>46</v>
       </c>
-      <c r="J1" t="s" s="0">
+      <c r="J1" t="s">
         <v>36</v>
       </c>
-      <c r="K1" t="s" s="0">
+      <c r="K1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0">
+      <c r="D2">
         <v>105369874</v>
       </c>
-      <c r="E2" s="0">
+      <c r="E2">
         <v>555551</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -702,24 +783,24 @@
       <c r="J2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K2" t="s" s="0">
+      <c r="K2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="0">
+      <c r="D3">
         <v>105369876</v>
       </c>
-      <c r="E3" s="0">
+      <c r="E3">
         <v>555553</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -737,24 +818,24 @@
       <c r="J3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K3" t="s" s="0">
+      <c r="K3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="0">
+      <c r="D4">
         <v>105369875</v>
       </c>
-      <c r="E4" s="0">
+      <c r="E4">
         <v>555552</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -772,24 +853,24 @@
       <c r="J4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K4" t="s" s="0">
+      <c r="K4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="0">
+      <c r="D5">
         <v>105369877</v>
       </c>
-      <c r="E5" s="0">
+      <c r="E5">
         <v>555554</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -807,24 +888,24 @@
       <c r="J5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K5" t="s" s="0">
+      <c r="K5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="0">
+      <c r="D6">
         <v>105369878</v>
       </c>
-      <c r="E6" s="0">
+      <c r="E6">
         <v>555555</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -842,24 +923,24 @@
       <c r="J6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K6" t="s" s="0">
+      <c r="K6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="0">
+      <c r="D7">
         <v>105369879</v>
       </c>
-      <c r="E7" s="0">
+      <c r="E7">
         <v>555556</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -877,24 +958,24 @@
       <c r="J7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K7" t="s" s="0">
-        <v>26</v>
+      <c r="K7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>50</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="0">
+      <c r="D8">
         <v>105369880</v>
       </c>
-      <c r="E8" s="0">
+      <c r="E8">
         <v>555557</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -912,24 +993,24 @@
       <c r="J8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K8" t="s" s="0">
-        <v>26</v>
+      <c r="K8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>67</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="0">
+      <c r="D9">
         <v>105369881</v>
       </c>
-      <c r="E9" s="0">
+      <c r="E9">
         <v>555558</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -947,24 +1028,24 @@
       <c r="J9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K9" t="s" s="0">
-        <v>26</v>
+      <c r="K9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s" s="0">
+      <c r="A10" t="s">
         <v>68</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" t="s" s="0">
+      <c r="C10" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="0">
+      <c r="D10">
         <v>105369882</v>
       </c>
-      <c r="E10" s="0">
+      <c r="E10">
         <v>555559</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -982,24 +1063,24 @@
       <c r="J10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K10" t="s" s="0">
+      <c r="K10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s" s="0">
+      <c r="A11" t="s">
         <v>69</v>
       </c>
-      <c r="B11" t="s" s="0">
+      <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" t="s" s="0">
+      <c r="C11" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="0">
+      <c r="D11">
         <v>105369883</v>
       </c>
-      <c r="E11" s="0">
+      <c r="E11">
         <v>555560</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -1017,24 +1098,24 @@
       <c r="J11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K11" t="s" s="0">
+      <c r="K11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s" s="0">
+      <c r="A12" t="s">
         <v>70</v>
       </c>
-      <c r="B12" t="s" s="0">
+      <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s" s="0">
+      <c r="C12" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="0">
+      <c r="D12">
         <v>105369884</v>
       </c>
-      <c r="E12" s="0">
+      <c r="E12">
         <v>555561</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -1052,24 +1133,24 @@
       <c r="J12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K12" t="s" s="0">
+      <c r="K12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s" s="0">
+      <c r="A13" t="s">
         <v>71</v>
       </c>
-      <c r="B13" t="s" s="0">
+      <c r="B13" t="s">
         <v>21</v>
       </c>
-      <c r="C13" t="s" s="0">
+      <c r="C13" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="0">
+      <c r="D13">
         <v>105369885</v>
       </c>
-      <c r="E13" s="0">
+      <c r="E13">
         <v>555562</v>
       </c>
       <c r="F13" s="1" t="s">
@@ -1087,7 +1168,322 @@
       <c r="J13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K13" t="s" s="0">
+      <c r="K13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>105369886</v>
+      </c>
+      <c r="E14">
+        <v>555563</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>105369887</v>
+      </c>
+      <c r="E15">
+        <v>555564</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>105369888</v>
+      </c>
+      <c r="E16">
+        <v>555565</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>105369889</v>
+      </c>
+      <c r="E17">
+        <v>555566</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18">
+        <v>105369890</v>
+      </c>
+      <c r="E18">
+        <v>555567</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>105369891</v>
+      </c>
+      <c r="E19">
+        <v>555568</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>105369892</v>
+      </c>
+      <c r="E20">
+        <v>555569</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21">
+        <v>105369893</v>
+      </c>
+      <c r="E21">
+        <v>555570</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>105369894</v>
+      </c>
+      <c r="E22">
+        <v>555571</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K22" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualizar archivo de datos Excel para reflejar cambios en la estructura de pruebas automatizadas.
</commit_message>
<xml_diff>
--- a/src/test/resources/datos.xlsx
+++ b/src/test/resources/datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jose.ladino\Automatizacion\ProjectMaven\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE042979-1C38-43BD-9B45-A9F67492C42C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44ACFFE-C9C2-4BF4-B966-8006E8452305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-1815" windowWidth="29040" windowHeight="15720" xr2:uid="{1B2942B2-1002-49AC-B066-AD15A2B34D50}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{1B2942B2-1002-49AC-B066-AD15A2B34D50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="98">
   <si>
     <t>Estado</t>
   </si>
@@ -130,9 +130,6 @@
   </si>
   <si>
     <t>2001-02-22</t>
-  </si>
-  <si>
-    <t>Usado</t>
   </si>
   <si>
     <t>Genero</t>
@@ -702,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55EA86F-2CF4-4D61-97BB-1D094DEA001F}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,13 +737,13 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K1" t="s">
         <v>0</v>
@@ -775,16 +772,16 @@
         <v>33</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -810,16 +807,16 @@
         <v>34</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -842,19 +839,19 @@
         <v>28</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -877,19 +874,19 @@
         <v>30</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K5" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -912,19 +909,19 @@
         <v>31</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K6" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -947,24 +944,24 @@
         <v>32</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -979,27 +976,27 @@
         <v>555557</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K8" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
@@ -1014,27 +1011,27 @@
         <v>555558</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K9" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -1049,19 +1046,19 @@
         <v>555559</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K10" t="s">
         <v>26</v>
@@ -1069,7 +1066,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
@@ -1084,19 +1081,19 @@
         <v>555560</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K11" t="s">
         <v>26</v>
@@ -1104,7 +1101,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
@@ -1119,19 +1116,19 @@
         <v>555561</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K12" t="s">
         <v>26</v>
@@ -1139,7 +1136,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
         <v>21</v>
@@ -1154,19 +1151,19 @@
         <v>555562</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K13" t="s">
         <v>26</v>
@@ -1174,7 +1171,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -1189,19 +1186,19 @@
         <v>555563</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K14" t="s">
         <v>26</v>
@@ -1209,7 +1206,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
@@ -1224,19 +1221,19 @@
         <v>555564</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K15" t="s">
         <v>26</v>
@@ -1244,7 +1241,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
@@ -1259,19 +1256,19 @@
         <v>555565</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K16" t="s">
         <v>26</v>
@@ -1279,7 +1276,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -1294,19 +1291,19 @@
         <v>555566</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K17" t="s">
         <v>26</v>
@@ -1314,7 +1311,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B18" t="s">
         <v>12</v>
@@ -1329,19 +1326,19 @@
         <v>555567</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K18" t="s">
         <v>26</v>
@@ -1349,7 +1346,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
@@ -1364,19 +1361,19 @@
         <v>555568</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K19" t="s">
         <v>26</v>
@@ -1384,7 +1381,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -1399,19 +1396,19 @@
         <v>555569</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K20" t="s">
         <v>26</v>
@@ -1419,7 +1416,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B21" t="s">
         <v>12</v>
@@ -1434,19 +1431,19 @@
         <v>555570</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K21" t="s">
         <v>26</v>
@@ -1454,7 +1451,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
@@ -1469,19 +1466,19 @@
         <v>555571</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K22" t="s">
         <v>26</v>

</xml_diff>